<commit_message>
Switched to a QCN-27D+ (with DC passthrough) for S band, and made the U and L band 1/4 wave lengths a bit more precise after getting precise lengths from Eric.
</commit_message>
<xml_diff>
--- a/eagle/oresat0-plusz-end-card-BOM.xlsx
+++ b/eagle/oresat0-plusz-end-card-BOM.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31" count="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23" count="23">
   <si>
     <t>Cnt</t>
   </si>
@@ -62,21 +62,6 @@
     <t>Digi-Key</t>
   </si>
   <si>
-    <t>CM1, CM2, CM3</t>
-  </si>
-  <si>
-    <t>Molex</t>
-  </si>
-  <si>
-    <t>73300-0020</t>
-  </si>
-  <si>
-    <t>SMPM Connector Plug, Male Pin 50Ohm Board Edge</t>
-  </si>
-  <si>
-    <t>WM10772-ND</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -98,19 +83,10 @@
     <t>Mini-Circuits</t>
   </si>
   <si>
-    <t>QCN-19+</t>
-  </si>
-  <si>
     <t>Power Splitter/Combiner, 2 Way-90°, 50Ω, 1100-1925 Mhz, LTCC </t>
   </si>
   <si>
     <t>Mouser</t>
-  </si>
-  <si>
-    <t>139-QCN-19</t>
-  </si>
-  <si>
-    <t>MEZZANINE</t>
   </si>
   <si>
     <t>QBA-07+</t>
@@ -220,7 +196,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -415,20 +391,28 @@
       <c r="A10">
         <v>3</v>
       </c>
-      <c r="B10" t="s">
-        <v>13</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>CM1, CM2, CM3</t>
+        </is>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" t="s">
-        <v>16</v>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Molex</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>73300-0020</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>SMPM Connector Plug, Male Pin 50Ohm Board Edge</t>
+        </is>
       </c>
       <c r="G10" t="s">
         <v>11</v>
@@ -436,8 +420,10 @@
       <c r="H10" t="s">
         <v>12</v>
       </c>
-      <c r="I10" t="s">
-        <v>17</v>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>WM10772-ND</t>
+        </is>
       </c>
     </row>
     <row r="11" spans="1:256">
@@ -471,10 +457,10 @@
         <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:256" ht="13.5">
@@ -566,13 +552,13 @@
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
@@ -581,7 +567,7 @@
         <v>12</v>
       </c>
       <c r="I14" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:256" ht="13.5">
@@ -628,34 +614,40 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>QCN-19+</t>
+        </is>
       </c>
       <c r="F16" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G16" t="s">
         <v>11</v>
       </c>
       <c r="H16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I16" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>139-QCN-19</t>
+        </is>
       </c>
     </row>
     <row r="18" spans="1:256">
       <c r="A18" s="0"/>
-      <c r="B18" s="4" t="s">
-        <v>29</v>
+      <c r="B18" s="4" t="inlineStr">
+        <is>
+          <t>MEZZANINE</t>
+        </is>
       </c>
     </row>
     <row r="19" spans="1:256">
@@ -718,7 +710,7 @@
         <v>11</v>
       </c>
       <c r="H20" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -739,13 +731,13 @@
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E21" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F21" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G21" t="s">
         <v>11</v>
@@ -754,7 +746,7 @@
         <v>12</v>
       </c>
       <c r="I21" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:256">
@@ -762,16 +754,16 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E22" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -782,10 +774,10 @@
         <v>11</v>
       </c>
       <c r="H22" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I22" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:256">
@@ -801,25 +793,25 @@
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>QCN-27+</t>
+          <t>QCN-27D+</t>
         </is>
       </c>
       <c r="F23" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G23" t="s">
         <v>11</v>
       </c>
       <c r="H23" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>139-QCN-27</t>
+          <t>139-QCN-27D</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Forgot to remove a meltwire resistor.
</commit_message>
<xml_diff>
--- a/eagle/oresat0-plusz-end-card-BOM.xlsx
+++ b/eagle/oresat0-plusz-end-card-BOM.xlsx
@@ -196,7 +196,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -572,11 +572,11 @@
     </row>
     <row r="15" spans="1:256" ht="13.5">
       <c r="A15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>R4, R5</t>
+          <t>R4</t>
         </is>
       </c>
       <c r="C15" t="s">

</xml_diff>

<commit_message>
Version 1.2 of the OreSat0 end card and mezzanine.
Largest change is the position of the antennas on the end card; changes to the deployer changed the antenna placement which triggered everything else.

Other changes include fiducials, attributes cleanup, move to 0603 resistors, and misc polish.
</commit_message>
<xml_diff>
--- a/eagle/oresat0-plusz-end-card-BOM.xlsx
+++ b/eagle/oresat0-plusz-end-card-BOM.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23" count="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24" count="24">
   <si>
     <t>Cnt</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>QBA-07+</t>
+  </si>
+  <si>
+    <t>139-QCN-27</t>
   </si>
 </sst>
 </file>
@@ -196,7 +199,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -256,7 +259,7 @@
     <row r="4" spans="1:256" customHeight="1" ht="12.75">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>PCB version: 1.1</t>
+          <t>PCB version: 1.2</t>
         </is>
       </c>
       <c r="B4" s="3"/>
@@ -589,12 +592,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>PAC100001008FA1000</t>
+          <t>PAC100007508FA1000</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Res 1 ohm 1W 1% Axial high temperature</t>
+          <t>Res 7.5 ohm 1W 1% Axial high temperature</t>
         </is>
       </c>
       <c r="G15" t="s">
@@ -797,11 +800,13 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>QCN-27D+</t>
-        </is>
-      </c>
-      <c r="F23" t="s">
-        <v>20</v>
+          <t>QCN-27+</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Power Splitter/Combiner, 2 Way-90°, 50Ω, 1700 to 2700 Mhz, LTCC </t>
+        </is>
       </c>
       <c r="G23" t="s">
         <v>11</v>
@@ -809,10 +814,8 @@
       <c r="H23" t="s">
         <v>21</v>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>139-QCN-27D</t>
-        </is>
+      <c r="I23" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:256" customHeight="1" ht="12.75">

</xml_diff>

<commit_message>
Fixed bad part number for end card to end cap connector.
</commit_message>
<xml_diff>
--- a/eagle/oresat0-plusz-end-card-BOM.xlsx
+++ b/eagle/oresat0-plusz-end-card-BOM.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24" count="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22" count="22">
   <si>
     <t>Cnt</t>
   </si>
@@ -83,16 +83,10 @@
     <t>Mini-Circuits</t>
   </si>
   <si>
-    <t>Power Splitter/Combiner, 2 Way-90°, 50Ω, 1100-1925 Mhz, LTCC </t>
-  </si>
-  <si>
     <t>Mouser</t>
   </si>
   <si>
     <t>QBA-07+</t>
-  </si>
-  <si>
-    <t>139-QCN-27</t>
   </si>
 </sst>
 </file>
@@ -199,7 +193,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
+      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -370,12 +364,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>M55-6021242R</t>
+          <t>M55-6001242R</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>CONN RCPT 12POS 0.05 GOLD SMD -- +Z End Cap connector</t>
+          <t>12 Position Receptacle Connector 0.050" (1.27mm) Surface Mount Gold</t>
         </is>
       </c>
       <c r="G9" t="s">
@@ -386,7 +380,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>952-3851-1-ND</t>
+          <t>952-3835-1-ND</t>
         </is>
       </c>
     </row>
@@ -630,14 +624,16 @@
           <t>QCN-19+</t>
         </is>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>20</v>
+      <c r="F16" s="5" t="inlineStr">
+        <is>
+          <t>Power Splitter/Combiner, 2 Way-90°, 50Ω, 1100-1925 Mhz, LTCC </t>
+        </is>
       </c>
       <c r="G16" t="s">
         <v>11</v>
       </c>
       <c r="H16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -713,7 +709,7 @@
         <v>11</v>
       </c>
       <c r="H20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -766,7 +762,7 @@
         <v>19</v>
       </c>
       <c r="E22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -780,7 +776,7 @@
         <v>19</v>
       </c>
       <c r="I22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:256">
@@ -812,10 +808,12 @@
         <v>11</v>
       </c>
       <c r="H23" t="s">
-        <v>21</v>
-      </c>
-      <c r="I23" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>139-QCN-27</t>
+        </is>
       </c>
     </row>
     <row r="24" spans="1:256" customHeight="1" ht="12.75">

</xml_diff>